<commit_message>
what appears to be a more recent version
</commit_message>
<xml_diff>
--- a/TechSpecs.xlsx
+++ b/TechSpecs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="9360" windowHeight="6360" tabRatio="729" activeTab="10"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="7080" windowHeight="3030" tabRatio="834"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="5" r:id="rId1"/>
@@ -18,13 +18,15 @@
     <sheet name="Entity" sheetId="9" r:id="rId9"/>
     <sheet name="Enemy" sheetId="10" r:id="rId10"/>
     <sheet name="Sheet1" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet2" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet3" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="321">
   <si>
     <t>call input</t>
   </si>
@@ -209,15 +211,6 @@
     <t>player</t>
   </si>
   <si>
-    <t>movement</t>
-  </si>
-  <si>
-    <t>attacks</t>
-  </si>
-  <si>
-    <t>dying effects</t>
-  </si>
-  <si>
     <t>updates every time</t>
   </si>
   <si>
@@ -248,18 +241,9 @@
     <t>x</t>
   </si>
   <si>
-    <t>animates</t>
-  </si>
-  <si>
-    <t>walk script/animation</t>
-  </si>
-  <si>
     <t>limited existance (time)</t>
   </si>
   <si>
-    <t>player object</t>
-  </si>
-  <si>
     <t>Map Object: updates with map</t>
   </si>
   <si>
@@ -299,9 +283,6 @@
     <t>money display</t>
   </si>
   <si>
-    <t>relies on something else</t>
-  </si>
-  <si>
     <t>touching an enemy hurts</t>
   </si>
   <si>
@@ -416,9 +397,6 @@
     <t>initializes and is responsible for updating them</t>
   </si>
   <si>
-    <t>direction facing</t>
-  </si>
-  <si>
     <t>frame order and time for each direction</t>
   </si>
   <si>
@@ -428,9 +406,6 @@
     <t>updates and renders with whomever's sprite it is</t>
   </si>
   <si>
-    <t>what if used flags to say 'moving left' then sprite class automatically goes through sequence of animations until flag is changed/turned off</t>
-  </si>
-  <si>
     <t xml:space="preserve">idea: what if there existed a position handler class.  </t>
   </si>
   <si>
@@ -473,9 +448,6 @@
     <t>for non-player:</t>
   </si>
   <si>
-    <t>Ideally handler should be usable by anybody and should not know whether it's parent is the player or not</t>
-  </si>
-  <si>
     <t>b) handler reports no collisions</t>
   </si>
   <si>
@@ -539,9 +511,6 @@
     <t>pos handler</t>
   </si>
   <si>
-    <t>ALL position related stuff, INCLUDING basic storing of x/y coordinates is handled by this</t>
-  </si>
-  <si>
     <t>knows nothing - information simply used by sprite</t>
   </si>
   <si>
@@ -566,21 +535,9 @@
     <t>?</t>
   </si>
   <si>
-    <t>player directly affects</t>
-  </si>
-  <si>
-    <t>player is affected by</t>
-  </si>
-  <si>
     <t>effect (ie. Explosion)</t>
   </si>
   <si>
-    <t>has hit points</t>
-  </si>
-  <si>
-    <t>has an element</t>
-  </si>
-  <si>
     <t>Control reader</t>
   </si>
   <si>
@@ -704,26 +661,341 @@
     <t>render with (after) map</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>built into tileset</t>
   </si>
   <si>
-    <t>player created block</t>
-  </si>
-  <si>
-    <t>pre-created block</t>
-  </si>
-  <si>
-    <t>act the same as spawningpoint/map switches/playerblocks?</t>
+    <t>Sprite Creator</t>
+  </si>
+  <si>
+    <t>Sprite base class</t>
+  </si>
+  <si>
+    <t>sprite meta data</t>
+  </si>
+  <si>
+    <t>gets frames</t>
+  </si>
+  <si>
+    <t>uses Frame class to get a full un-parsed list of sprites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this will contain animation data using frames </t>
+  </si>
+  <si>
+    <t>ties frames and meta data together</t>
+  </si>
+  <si>
+    <t>animation data will be in the form of a dict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left: </t>
+  </si>
+  <si>
+    <t>frame3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait 3 </t>
+  </si>
+  <si>
+    <t>frame 4</t>
+  </si>
+  <si>
+    <t>wait 3</t>
+  </si>
+  <si>
+    <t>frame 3</t>
+  </si>
+  <si>
+    <t>frame 5</t>
+  </si>
+  <si>
+    <t>Right:</t>
+  </si>
+  <si>
+    <t>frame 6</t>
+  </si>
+  <si>
+    <t>frame 7</t>
+  </si>
+  <si>
+    <t>frame 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> function not a class</t>
+  </si>
+  <si>
+    <t>will need to be defined manually for every new entity</t>
+  </si>
+  <si>
+    <t>pros:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons: </t>
+  </si>
+  <si>
+    <t>a bit less efficient during runtime</t>
+  </si>
+  <si>
+    <t>could just have essentially all possible states for every sprite, but would need to verify actual existence before using</t>
+  </si>
+  <si>
+    <t>much easier in the long run</t>
+  </si>
+  <si>
+    <t>would accept meta data as an initial argument</t>
+  </si>
+  <si>
+    <t>visual</t>
+  </si>
+  <si>
+    <t>character in open:</t>
+  </si>
+  <si>
+    <t>character with shallow ceiling:</t>
+  </si>
+  <si>
+    <t>creates next to character in direction character facing</t>
+  </si>
+  <si>
+    <t>block will fall down a pit if this is 'correct' position</t>
+  </si>
+  <si>
+    <t>character facing wall:</t>
+  </si>
+  <si>
+    <t>created block will push the character back</t>
+  </si>
+  <si>
+    <t>creates as normal</t>
+  </si>
+  <si>
+    <t>To pick up a block:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">presently not an option </t>
+  </si>
+  <si>
+    <t>character in ditch:</t>
+  </si>
+  <si>
+    <t>block will be created underneath the character</t>
+  </si>
+  <si>
+    <t>technical</t>
+  </si>
+  <si>
+    <t>get direction player is facing</t>
+  </si>
+  <si>
+    <t>if left:</t>
+  </si>
+  <si>
+    <t>if right:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">player.y + block.h </t>
+  </si>
+  <si>
+    <t xml:space="preserve">player.x + player.HotX - block.w </t>
+  </si>
+  <si>
+    <t xml:space="preserve">player.x + player.HotX + player.HotW </t>
+  </si>
+  <si>
+    <t>IF there's a problem with edges lining up… there shouldn't be because block.hotX/Y starts at 1, not 0</t>
+  </si>
+  <si>
+    <t>this can afford to be a bit less specific in starting location</t>
+  </si>
+  <si>
+    <t>adjust block to the right (opposite of player) until block is no longer on the wall.</t>
+  </si>
+  <si>
+    <t>track how much the adjustment was and make player move same distance</t>
+  </si>
+  <si>
+    <t>block moves down to below slope</t>
+  </si>
+  <si>
+    <t>block moves up to rest on slope</t>
+  </si>
+  <si>
+    <t>To make a block:</t>
+  </si>
+  <si>
+    <t>take same, but opposite actions as when facing left</t>
+  </si>
+  <si>
+    <t>same as others</t>
+  </si>
+  <si>
+    <t>character checks whether there is at least one non-obstructed tile next to him in all 4 quadrants -&gt;</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Obstructed</t>
+  </si>
+  <si>
+    <t>If and only if all 4 quadrants are obstructed:</t>
+  </si>
+  <si>
+    <t>block created at:</t>
+  </si>
+  <si>
+    <t>player.x + player.hotX</t>
+  </si>
+  <si>
+    <t>player.y + player.hotY - block.height</t>
+  </si>
+  <si>
+    <t>player is displaced to on top of the block</t>
+  </si>
+  <si>
+    <t>If not, other rules will go into effect</t>
+  </si>
+  <si>
+    <t>In the unseemly event the player is completely closed in:</t>
+  </si>
+  <si>
+    <t>The block will not be created and it will be up to the human to reset the level.</t>
+  </si>
+  <si>
+    <t>No block made</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>block would be as in ©:</t>
+  </si>
+  <si>
+    <t>block would be as in (B):</t>
+  </si>
+  <si>
+    <t>SUMMARY:</t>
+  </si>
+  <si>
+    <t>Check first whether either of the two quadrants in the direction the player is facing are open.</t>
+  </si>
+  <si>
+    <t>If not:</t>
+  </si>
+  <si>
+    <t>check if either of the two quadrants behind the player are open</t>
+  </si>
+  <si>
+    <t>If so:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> make block at head height, or, if one is closed, inside the one that is closed.</t>
+  </si>
+  <si>
+    <t>make block at head height, or in quadrant that is open.</t>
+  </si>
+  <si>
+    <t>Check if space above player is obstructed:</t>
+  </si>
+  <si>
+    <t>Do nothing</t>
+  </si>
+  <si>
+    <t>Make a block below the player and, hopefully, let the player rise naturally on top of block.</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when making a block, try to make it as close to the player as possible… </t>
+  </si>
+  <si>
+    <t>but the quadrant needs to be open anyway since they cannot both share a single tile wholely</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>will obstruct movement</t>
+  </si>
+  <si>
+    <t>walls</t>
+  </si>
+  <si>
+    <t>base sprite class and inheret for different types of sprites, say, stationary vs. not</t>
+  </si>
+  <si>
+    <t>uses flags (states) to say 'moving left'</t>
+  </si>
+  <si>
+    <t>sprite class automatically goes through sequence of animations until flag is changed/turned off</t>
+  </si>
+  <si>
+    <t>return the item</t>
+  </si>
+  <si>
+    <t>handler must be usable by anybody and should not know whether it's parent is the player or not</t>
+  </si>
+  <si>
+    <t>ALL movement related stuff. Does NOT store x/y/sizes since that info is needed by other stuff</t>
+  </si>
+  <si>
+    <t>otherstuff should not have to look down to retrieve it</t>
+  </si>
+  <si>
+    <t>has hit points (Entity)</t>
+  </si>
+  <si>
+    <t>has an element (Element)</t>
+  </si>
+  <si>
+    <t>movement (Position Handler)</t>
+  </si>
+  <si>
+    <t>attacks (Sprite, Collisions)</t>
+  </si>
+  <si>
+    <t>animates (Sprite)</t>
+  </si>
+  <si>
+    <t>dying effects (Sprite)</t>
+  </si>
+  <si>
+    <t>player directly affects (Box)</t>
+  </si>
+  <si>
+    <t>player is affected by (Box)</t>
+  </si>
+  <si>
+    <t>walk script/ AI (new class)</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>has gravity (Position Handler)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -753,8 +1025,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -779,6 +1058,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -792,7 +1083,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -815,6 +1106,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment textRotation="135"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,8 +1127,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AB36" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:AB36">
-    <filterColumn colId="7"/>
+    <filterColumn colId="2"/>
     <filterColumn colId="12"/>
+    <filterColumn colId="14"/>
     <filterColumn colId="15"/>
     <filterColumn colId="16"/>
     <filterColumn colId="17"/>
@@ -849,33 +1146,33 @@
   </autoFilter>
   <tableColumns count="28">
     <tableColumn id="1" name="Object Name"/>
-    <tableColumn id="3" name="movement"/>
-    <tableColumn id="4" name="attacks"/>
-    <tableColumn id="5" name="animates"/>
-    <tableColumn id="6" name="dying effects"/>
+    <tableColumn id="3" name="movement (Position Handler)"/>
+    <tableColumn id="8" name="has gravity (Position Handler)"/>
+    <tableColumn id="4" name="attacks (Sprite, Collisions)"/>
+    <tableColumn id="5" name="animates (Sprite)"/>
+    <tableColumn id="6" name="dying effects (Sprite)"/>
     <tableColumn id="7" name="limited existance (time)"/>
     <tableColumn id="9" name="updates every time"/>
+    <tableColumn id="10" name="has hit points (Entity)"/>
+    <tableColumn id="11" name="has an element (Element)"/>
+    <tableColumn id="12" name="other stats"/>
+    <tableColumn id="13" name="player directly affects (Box)"/>
+    <tableColumn id="28" name="player is affected by (Box)"/>
+    <tableColumn id="14" name="walk script/ AI (new class)"/>
     <tableColumn id="20" name="do NOT update"/>
-    <tableColumn id="10" name="has hit points"/>
-    <tableColumn id="11" name="has an element"/>
-    <tableColumn id="12" name="other stats"/>
-    <tableColumn id="13" name="player directly affects"/>
-    <tableColumn id="28" name="player is affected by"/>
-    <tableColumn id="14" name="walk script/animation"/>
-    <tableColumn id="15" name="player object"/>
     <tableColumn id="22" name="Map Object"/>
     <tableColumn id="2" name="built into tileset"/>
+    <tableColumn id="21" name="render with (after) map"/>
     <tableColumn id="16" name="updates with map"/>
-    <tableColumn id="21" name="render with (after) map"/>
     <tableColumn id="17" name="Entity"/>
     <tableColumn id="18" name="effect"/>
     <tableColumn id="19" name="object"/>
-    <tableColumn id="23" name="relies on something else"/>
     <tableColumn id="24" name="needs sprite handler"/>
     <tableColumn id="25" name="needs input"/>
     <tableColumn id="26" name="uses real x/y"/>
     <tableColumn id="27" name="uses map x/y"/>
-    <tableColumn id="8" name="Column1"/>
+    <tableColumn id="29" name="will obstruct movement"/>
+    <tableColumn id="30" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1168,112 +1465,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" customWidth="1"/>
-    <col min="9" max="12" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5" customWidth="1"/>
-    <col min="14" max="16" width="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="5" customWidth="1"/>
-    <col min="19" max="19" width="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5" customWidth="1"/>
-    <col min="21" max="28" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="14" width="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5" customWidth="1"/>
+    <col min="17" max="18" width="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5" customWidth="1"/>
+    <col min="21" max="31" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="7" customFormat="1" ht="93.75">
+    <row r="1" spans="1:29" s="7" customFormat="1" ht="110.25">
       <c r="A1" s="9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="I1" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="8" t="s">
+      <c r="W1" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z1" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>194</v>
-      </c>
       <c r="AA1" s="7" t="s">
-        <v>195</v>
+        <v>301</v>
       </c>
       <c r="AB1" s="7" t="s">
-        <v>226</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:29">
@@ -1281,333 +1574,346 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N2" t="s">
-        <v>73</v>
-      </c>
-      <c r="O2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="T2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="W2" t="s">
+        <v>70</v>
       </c>
       <c r="X2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Y2" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>73</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="AA2" s="7"/>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>70</v>
       </c>
       <c r="I3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="T3" t="s">
-        <v>73</v>
-      </c>
-      <c r="X3" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="W3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" t="s">
+        <v>70</v>
       </c>
       <c r="L4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="R4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="T4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="M5" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="O5" t="s">
+        <v>70</v>
       </c>
       <c r="P5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q5" t="s">
-        <v>73</v>
-      </c>
-      <c r="S5" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="R5" t="s">
+        <v>70</v>
       </c>
       <c r="V5" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>70</v>
       </c>
       <c r="AC5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" t="s">
+        <v>70</v>
+      </c>
+      <c r="P6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>70</v>
+      </c>
+      <c r="R6" t="s">
+        <v>70</v>
+      </c>
+      <c r="V6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC6" t="s">
         <v>73</v>
-      </c>
-      <c r="L6" t="s">
-        <v>73</v>
-      </c>
-      <c r="P6" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>73</v>
-      </c>
-      <c r="S6" t="s">
-        <v>73</v>
-      </c>
-      <c r="V6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="H7" t="s">
+        <v>70</v>
       </c>
       <c r="L7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V7" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>70</v>
       </c>
       <c r="AC7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="L8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M8" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="O8" t="s">
+        <v>70</v>
       </c>
       <c r="P8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q8" t="s">
-        <v>73</v>
-      </c>
-      <c r="S8" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="R8" t="s">
+        <v>70</v>
       </c>
       <c r="V8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>70</v>
       </c>
       <c r="AC8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B9" t="s">
-        <v>230</v>
+        <v>319</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" t="s">
+        <v>70</v>
       </c>
       <c r="L9" t="s">
-        <v>73</v>
-      </c>
-      <c r="S9" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="T9" t="s">
+        <v>70</v>
+      </c>
+      <c r="W9" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" s="6" t="s">
-        <v>228</v>
+        <v>169</v>
+      </c>
+      <c r="B10" t="s">
+        <v>168</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10" t="s">
-        <v>73</v>
-      </c>
-      <c r="J10" t="s">
-        <v>73</v>
-      </c>
-      <c r="L10" t="s">
-        <v>73</v>
-      </c>
-      <c r="T10" t="s">
-        <v>73</v>
-      </c>
-      <c r="X10" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="H10" t="s">
+        <v>70</v>
+      </c>
+      <c r="U10" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="6" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" t="s">
-        <v>73</v>
-      </c>
-      <c r="U11" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="H11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" t="s">
-        <v>73</v>
-      </c>
-      <c r="M12" t="s">
-        <v>73</v>
+        <v>302</v>
+      </c>
+      <c r="O12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:29">
@@ -1615,10 +1921,9 @@
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -1642,61 +1947,50 @@
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
-      <c r="AA14" s="12"/>
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="W15" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>73</v>
+        <v>82</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="W16" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28">
+        <v>83</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
       <c r="A17" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="W17" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28">
+        <v>84</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28">
+        <v>101</v>
+      </c>
+      <c r="G18" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
       <c r="A20" s="12" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
@@ -1717,88 +2011,86 @@
       <c r="U20" s="12"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="12" t="s">
-        <v>73</v>
-      </c>
+      <c r="X20" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
-      <c r="AA20" s="12"/>
-    </row>
-    <row r="21" spans="1:28">
+    </row>
+    <row r="21" spans="1:26">
       <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" t="s">
         <v>102</v>
       </c>
-      <c r="B21" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28">
+      <c r="X21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
       <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="X22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26">
+      <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" t="s">
+        <v>102</v>
+      </c>
+      <c r="X23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
+      <c r="A24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" t="s">
         <v>103</v>
       </c>
-      <c r="B22" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28">
-      <c r="A23" t="s">
+      <c r="X24" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" t="s">
+        <v>103</v>
+      </c>
+      <c r="X25" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26">
+      <c r="A26" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
+      <c r="A28" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B23" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28">
-      <c r="A24" t="s">
-        <v>105</v>
-      </c>
-      <c r="B24" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28">
-      <c r="A25" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28">
-      <c r="A26" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28">
-      <c r="A28" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -1820,22 +2112,20 @@
       <c r="X28" s="10"/>
       <c r="Y28" s="10"/>
       <c r="Z28" s="10"/>
-      <c r="AA28" s="10"/>
-    </row>
-    <row r="29" spans="1:28">
+    </row>
+    <row r="29" spans="1:26">
       <c r="A29" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="10"/>
+        <v>105</v>
+      </c>
       <c r="D29" s="10"/>
-      <c r="E29" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="H29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
@@ -1854,22 +2144,20 @@
       <c r="X29" s="10"/>
       <c r="Y29" s="10"/>
       <c r="Z29" s="10"/>
-      <c r="AA29" s="10"/>
-    </row>
-    <row r="30" spans="1:28">
+    </row>
+    <row r="30" spans="1:26">
       <c r="A30" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" s="10"/>
+        <v>106</v>
+      </c>
       <c r="D30" s="10"/>
-      <c r="E30" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="H30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -1888,11 +2176,10 @@
       <c r="X30" s="10"/>
       <c r="Y30" s="10"/>
       <c r="Z30" s="10"/>
-      <c r="AA30" s="10"/>
-    </row>
-    <row r="31" spans="1:28">
+    </row>
+    <row r="31" spans="1:26">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -1918,14 +2205,11 @@
       <c r="X31" s="10"/>
       <c r="Y31" s="10"/>
       <c r="Z31" s="10"/>
-      <c r="AA31" s="10"/>
-      <c r="AB31" s="10"/>
-    </row>
-    <row r="32" spans="1:28">
+    </row>
+    <row r="32" spans="1:26">
       <c r="A32" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" s="10"/>
+        <v>108</v>
+      </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -1937,6 +2221,7 @@
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
       <c r="R32" s="10"/>
@@ -1948,34 +2233,33 @@
       <c r="X32" s="10"/>
       <c r="Y32" s="10"/>
       <c r="Z32" s="10"/>
-      <c r="AA32" s="10"/>
-    </row>
-    <row r="34" spans="1:5">
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="E37" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="E38" t="s">
-        <v>93</v>
+    <row r="37" spans="1:6">
+      <c r="F37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="F38" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1999,42 +2283,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2046,7 +2330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2054,22 +2338,657 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="C6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="D7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="D8" t="s">
+        <v>220</v>
+      </c>
+      <c r="E8" t="s">
+        <v>221</v>
+      </c>
+      <c r="F8" t="s">
+        <v>222</v>
+      </c>
+      <c r="G8" t="s">
+        <v>223</v>
+      </c>
+      <c r="H8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J8" t="s">
+        <v>224</v>
+      </c>
+      <c r="K8" t="s">
+        <v>226</v>
+      </c>
+      <c r="L8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="D9" t="s">
+        <v>227</v>
+      </c>
+      <c r="E9" t="s">
+        <v>228</v>
+      </c>
+      <c r="F9" t="s">
+        <v>222</v>
+      </c>
+      <c r="G9" t="s">
+        <v>229</v>
+      </c>
+      <c r="H9" t="s">
+        <v>224</v>
+      </c>
+      <c r="I9" t="s">
+        <v>229</v>
+      </c>
+      <c r="J9" t="s">
+        <v>224</v>
+      </c>
+      <c r="K9" t="s">
+        <v>230</v>
+      </c>
+      <c r="L9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" t="s">
+        <v>218</v>
+      </c>
+      <c r="G10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="C11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="D12" t="s">
+        <v>233</v>
+      </c>
+      <c r="E12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="D13" t="s">
+        <v>234</v>
+      </c>
+      <c r="E13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q82"/>
+  <sheetViews>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="13" max="13" width="7.5703125" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" customWidth="1"/>
+    <col min="15" max="16" width="3.85546875" customWidth="1"/>
+    <col min="17" max="17" width="4.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="C4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2"/>
+      <c r="C7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="C12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="C14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="C16" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="B19" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="B24" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="C25" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="C26" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="B27" s="2"/>
+      <c r="D27" t="s">
+        <v>256</v>
+      </c>
+      <c r="H27" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28" s="2"/>
+      <c r="D28" t="s">
+        <v>255</v>
+      </c>
+      <c r="G28" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" s="2"/>
+      <c r="C29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="D30" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="D31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17">
+      <c r="B33" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17">
+      <c r="C34" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17">
+      <c r="D35" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17">
+      <c r="E36" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17">
+      <c r="E37" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17">
+      <c r="D38" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17">
+      <c r="C39" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17">
+      <c r="D40" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17">
+      <c r="E41" t="s">
+        <v>265</v>
+      </c>
+      <c r="N41" s="6"/>
+      <c r="O41" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q41" s="6"/>
+    </row>
+    <row r="42" spans="2:17">
+      <c r="D42" t="s">
+        <v>255</v>
+      </c>
+      <c r="M42" t="s">
+        <v>280</v>
+      </c>
+      <c r="N42" s="14"/>
+      <c r="O42" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="14"/>
+    </row>
+    <row r="43" spans="2:17">
+      <c r="N43" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="14"/>
+    </row>
+    <row r="44" spans="2:17">
+      <c r="B44" t="s">
+        <v>241</v>
+      </c>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+    </row>
+    <row r="45" spans="2:17">
+      <c r="C45" t="s">
+        <v>266</v>
+      </c>
+      <c r="N45" s="6"/>
+      <c r="Q45" s="6"/>
+    </row>
+    <row r="46" spans="2:17">
+      <c r="M46" t="s">
+        <v>281</v>
+      </c>
+      <c r="N46" s="17">
+        <v>1</v>
+      </c>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17">
+      <c r="B47" t="s">
+        <v>249</v>
+      </c>
+      <c r="N47" s="16">
+        <v>2</v>
+      </c>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17">
+      <c r="C48" t="s">
+        <v>267</v>
+      </c>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+    </row>
+    <row r="49" spans="3:17">
+      <c r="C49" t="s">
+        <v>271</v>
+      </c>
+      <c r="N49" s="6"/>
+      <c r="Q49" s="6"/>
+    </row>
+    <row r="50" spans="3:17">
+      <c r="D50" t="s">
+        <v>272</v>
+      </c>
+      <c r="M50" t="s">
+        <v>282</v>
+      </c>
+      <c r="N50" s="14"/>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="14"/>
+    </row>
+    <row r="51" spans="3:17">
+      <c r="E51" t="s">
+        <v>273</v>
+      </c>
+      <c r="N51" s="6"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="14"/>
+    </row>
+    <row r="52" spans="3:17">
+      <c r="E52" t="s">
+        <v>274</v>
+      </c>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
+    </row>
+    <row r="53" spans="3:17">
+      <c r="D53" t="s">
+        <v>275</v>
+      </c>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+    </row>
+    <row r="54" spans="3:17">
+      <c r="C54" t="s">
+        <v>276</v>
+      </c>
+      <c r="M54" t="s">
+        <v>283</v>
+      </c>
+      <c r="N54" s="14"/>
+      <c r="O54" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="14"/>
+    </row>
+    <row r="55" spans="3:17">
+      <c r="C55" t="s">
+        <v>277</v>
+      </c>
+      <c r="N55" s="14"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="14"/>
+    </row>
+    <row r="56" spans="3:17">
+      <c r="D56" t="s">
+        <v>278</v>
+      </c>
+      <c r="N56" s="14"/>
+      <c r="O56" s="15"/>
+      <c r="P56" s="15"/>
+      <c r="Q56" s="14"/>
+    </row>
+    <row r="57" spans="3:17">
+      <c r="N57" s="14"/>
+      <c r="O57" s="14"/>
+      <c r="P57" s="14"/>
+      <c r="Q57" s="14"/>
+    </row>
+    <row r="58" spans="3:17">
+      <c r="N58" s="6"/>
+      <c r="O58" s="6"/>
+      <c r="P58" s="6"/>
+      <c r="Q58" s="6"/>
+    </row>
+    <row r="60" spans="3:17" hidden="1"/>
+    <row r="61" spans="3:17">
+      <c r="N61" s="6"/>
+      <c r="Q61" s="6"/>
+    </row>
+    <row r="62" spans="3:17">
+      <c r="M62" t="s">
+        <v>284</v>
+      </c>
+      <c r="N62" s="6"/>
+      <c r="O62" s="15"/>
+      <c r="P62" s="15"/>
+      <c r="Q62" s="14"/>
+    </row>
+    <row r="63" spans="3:17">
+      <c r="N63" s="6"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="15"/>
+      <c r="Q63" s="14"/>
+    </row>
+    <row r="64" spans="3:17">
+      <c r="N64" s="14"/>
+      <c r="O64" s="14"/>
+      <c r="P64" s="14"/>
+      <c r="Q64" s="14"/>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="C66" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="C67" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="D68" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="C69" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="D70" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="D71" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="E72" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="D73" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="E74" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="E75" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6">
+      <c r="F76" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6">
+      <c r="E77" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="F78" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6">
+      <c r="C80" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4">
+      <c r="D81" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4">
+      <c r="D82" t="s">
+        <v>299</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2188,7 +3107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2440,17 +3359,17 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2462,92 +3381,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:F35"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D5" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D6" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="E7" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="F8" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="F9" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="C15" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2557,77 +3476,77 @@
     </row>
     <row r="20" spans="1:5">
       <c r="C20" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="C21" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="D22" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="E23" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="D24" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="E25" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="E26" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="D27" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="E28" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="C31" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="D32" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="C34" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="C35" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2647,52 +3566,52 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2702,170 +3621,181 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I34"/>
+  <dimension ref="A3:M38"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>130</v>
-      </c>
-    </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>135</v>
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="B12" t="s">
-        <v>136</v>
+      <c r="A12" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="B13" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="C14" t="s">
-        <v>138</v>
+      <c r="B14" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="B15" t="s">
-        <v>139</v>
+      <c r="C15" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="2:9">
-      <c r="C18" t="s">
-        <v>144</v>
-      </c>
-      <c r="D18" t="s">
-        <v>145</v>
+      <c r="B18" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="2:9">
       <c r="C19" t="s">
-        <v>142</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>146</v>
+        <v>135</v>
+      </c>
+      <c r="D19" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="2:9">
       <c r="C20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="C21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="D22" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="C27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="C29" t="s">
         <v>143</v>
-      </c>
-      <c r="D20" t="s">
-        <v>148</v>
-      </c>
-      <c r="F20" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9">
-      <c r="D21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9">
-      <c r="B23" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9">
-      <c r="B25" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9">
-      <c r="C26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9">
-      <c r="B27" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9">
-      <c r="C28" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9">
-      <c r="B30" t="s">
-        <v>168</v>
-      </c>
-      <c r="C30" t="s">
-        <v>169</v>
-      </c>
-      <c r="I30" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="31" spans="2:9">
       <c r="B31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" t="s">
+        <v>159</v>
+      </c>
+      <c r="I31" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" t="s">
         <v>59</v>
       </c>
-      <c r="C31" t="s">
-        <v>167</v>
-      </c>
-      <c r="F31" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7">
-      <c r="B33" t="s">
-        <v>170</v>
-      </c>
-      <c r="C33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7">
+      <c r="C32" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="B34" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C34" t="s">
-        <v>175</v>
-      </c>
-      <c r="G34" t="s">
-        <v>176</v>
+        <v>308</v>
+      </c>
+      <c r="M34" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="B35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" t="s">
+        <v>164</v>
+      </c>
+      <c r="G35" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2885,15 +3815,15 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2903,45 +3833,45 @@
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>